<commit_message>
time records as of 11/04/2021
</commit_message>
<xml_diff>
--- a/time-records/Lorenz-Oberhammer.xlsx
+++ b/time-records/Lorenz-Oberhammer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QE\Documents\Work\Nabu\03_Teaching\02_Courses\Software Engineering\SS21\Templates - Projektabwicklung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEA942A2-AB73-4044-A417-61D44F6F4FC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{748EA032-911B-4D5E-8026-C038D7C2F5AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28425" yWindow="4020" windowWidth="28245" windowHeight="17565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
   <si>
     <t>Datum</t>
   </si>
@@ -568,8 +568,8 @@
   <dimension ref="A1:D1011"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -1041,14 +1041,30 @@
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="8"/>
-      <c r="B34" s="7"/>
+      <c r="A34" s="8">
+        <v>44296</v>
+      </c>
+      <c r="B34" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="8"/>
-      <c r="B35" s="7"/>
-      <c r="D35" s="3"/>
+      <c r="A35" s="8">
+        <v>44297</v>
+      </c>
+      <c r="B35" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="8"/>

</xml_diff>

<commit_message>
ui for configuration of TimeFlip device
</commit_message>
<xml_diff>
--- a/time-records/Lorenz-Oberhammer.xlsx
+++ b/time-records/Lorenz-Oberhammer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24004"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24020"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QE\Documents\Work\Nabu\03_Teaching\02_Courses\Software Engineering\SS21\Templates - Projektabwicklung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{748EA032-911B-4D5E-8026-C038D7C2F5AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{57C44BCA-C129-41D5-8B1F-EA99CD80C73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28425" yWindow="4020" windowWidth="28245" windowHeight="17565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="38">
   <si>
     <t>Datum</t>
   </si>
@@ -138,7 +138,10 @@
     <t>Websockets</t>
   </si>
   <si>
-    <t>REST API + Refactoring</t>
+    <t>Zuweisung von Würfelseiten</t>
+  </si>
+  <si>
+    <t>Raspberry Pi</t>
   </si>
   <si>
     <t>ID</t>
@@ -565,11 +568,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F855F84B-A166-7442-8B83-EBB2C6A67214}">
-  <dimension ref="A1:D1011"/>
+  <dimension ref="A1:D1016"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="D47" sqref="D47"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -1037,7 +1040,7 @@
         <v>21</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1067,59 +1070,152 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="8"/>
-      <c r="B36" s="7"/>
+      <c r="A36" s="8">
+        <v>44298</v>
+      </c>
+      <c r="B36" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="8"/>
-      <c r="B37" s="7"/>
-      <c r="D37" s="3"/>
+      <c r="A37" s="8">
+        <v>44300</v>
+      </c>
+      <c r="B37" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="8"/>
-      <c r="B38" s="7"/>
+      <c r="A38" s="8">
+        <v>44301</v>
+      </c>
+      <c r="B38" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
-      <c r="D39" s="3"/>
+      <c r="A39" s="8">
+        <v>44303</v>
+      </c>
+      <c r="B39" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="8"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="8">
+        <v>44303</v>
+      </c>
+      <c r="B40" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="8"/>
-      <c r="B41" s="7"/>
-      <c r="D41" s="3"/>
+      <c r="A41" s="8">
+        <v>44305</v>
+      </c>
+      <c r="B41" s="7">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="8"/>
-      <c r="B42" s="7"/>
-      <c r="D42" s="3"/>
+      <c r="A42" s="8">
+        <v>44306</v>
+      </c>
+      <c r="B42" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="8"/>
-      <c r="B43" s="7"/>
-      <c r="D43" s="3"/>
+      <c r="A43" s="8">
+        <v>44307</v>
+      </c>
+      <c r="B43" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="8"/>
-      <c r="B44" s="7"/>
-      <c r="D44" s="3"/>
+      <c r="A44" s="8">
+        <v>44307</v>
+      </c>
+      <c r="B44" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="8"/>
-      <c r="B45" s="7"/>
-      <c r="D45" s="3"/>
+      <c r="A45" s="8">
+        <v>44310</v>
+      </c>
+      <c r="B45" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="8"/>
-      <c r="B46" s="7"/>
-      <c r="D46" s="3"/>
+      <c r="A46" s="8">
+        <v>44311</v>
+      </c>
+      <c r="B46" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="8"/>
@@ -5942,7 +6038,32 @@
       <c r="D1010" s="3"/>
     </row>
     <row r="1011" spans="1:4">
-      <c r="A1011" s="2"/>
+      <c r="A1011" s="8"/>
+      <c r="B1011" s="7"/>
+      <c r="D1011" s="3"/>
+    </row>
+    <row r="1012" spans="1:4">
+      <c r="A1012" s="8"/>
+      <c r="B1012" s="7"/>
+      <c r="D1012" s="3"/>
+    </row>
+    <row r="1013" spans="1:4">
+      <c r="A1013" s="8"/>
+      <c r="B1013" s="7"/>
+      <c r="D1013" s="3"/>
+    </row>
+    <row r="1014" spans="1:4">
+      <c r="A1014" s="8"/>
+      <c r="B1014" s="7"/>
+      <c r="D1014" s="3"/>
+    </row>
+    <row r="1015" spans="1:4">
+      <c r="A1015" s="8"/>
+      <c r="B1015" s="7"/>
+      <c r="D1015" s="3"/>
+    </row>
+    <row r="1016" spans="1:4">
+      <c r="A1016" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5954,7 +6075,7 @@
           <x14:formula1>
             <xm:f>Tätigkeiten!$B$2:$B$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1010</xm:sqref>
+          <xm:sqref>C2:C1015</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5975,10 +6096,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6002,7 +6123,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6010,7 +6131,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6018,7 +6139,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6050,7 +6171,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2">

</xml_diff>

<commit_message>
don't touch my time records
</commit_message>
<xml_diff>
--- a/time-records/Lorenz-Oberhammer.xlsx
+++ b/time-records/Lorenz-Oberhammer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QE\Documents\Work\Nabu\03_Teaching\02_Courses\Software Engineering\SS21\Templates - Projektabwicklung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3D190CD-B7C9-42FF-8143-A1140D1D9257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{57C44BCA-C129-41D5-8B1F-EA99CD80C73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28425" yWindow="4020" windowWidth="28245" windowHeight="17565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="38">
   <si>
     <t>Datum</t>
   </si>
@@ -572,7 +572,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C36" sqref="C36"/>
+      <selection pane="bottomRight" activeCell="D47" sqref="D47"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -1204,9 +1204,18 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="8"/>
-      <c r="B46" s="7"/>
-      <c r="D46" s="3"/>
+      <c r="A46" s="8">
+        <v>44311</v>
+      </c>
+      <c r="B46" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="8"/>

</xml_diff>

<commit_message>
make raspberry pi code more robust
</commit_message>
<xml_diff>
--- a/time-records/Lorenz-Oberhammer.xlsx
+++ b/time-records/Lorenz-Oberhammer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QE\Documents\Work\Nabu\03_Teaching\02_Courses\Software Engineering\SS21\Templates - Projektabwicklung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3E83EB0-F8CA-4A7C-BEDF-62A912B8E193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC9B9862-AE6E-4451-90EE-716A8A1279D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28425" yWindow="4020" windowWidth="28245" windowHeight="17565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
     <sheet name="Tätigkeiten" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="42">
   <si>
     <t>Datum</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>Issue Nr. 76</t>
+  </si>
+  <si>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t>Installationsskript Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Issue Nr. 68</t>
   </si>
   <si>
     <t>ID</t>
@@ -571,11 +580,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F855F84B-A166-7442-8B83-EBB2C6A67214}">
-  <dimension ref="A1:D1015"/>
+  <dimension ref="A1:D1016"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A51" sqref="A51:XFD51"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B58" sqref="B58"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -1301,34 +1310,88 @@
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="8"/>
-      <c r="B53" s="7"/>
-      <c r="D53" s="3"/>
+      <c r="A53" s="8">
+        <v>44318</v>
+      </c>
+      <c r="B53" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="8"/>
-      <c r="B54" s="7"/>
-      <c r="D54" s="3"/>
+      <c r="A54" s="8">
+        <v>44320</v>
+      </c>
+      <c r="B54" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="8"/>
-      <c r="B55" s="7"/>
-      <c r="D55" s="3"/>
+      <c r="A55" s="8">
+        <v>44322</v>
+      </c>
+      <c r="B55" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="8"/>
-      <c r="B56" s="7"/>
-      <c r="D56" s="3"/>
+      <c r="A56" s="8">
+        <v>44322</v>
+      </c>
+      <c r="B56" s="7">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="8"/>
-      <c r="B57" s="7"/>
-      <c r="D57" s="3"/>
+      <c r="A57" s="8">
+        <v>44324</v>
+      </c>
+      <c r="B57" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C57" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="8"/>
-      <c r="B58" s="7"/>
-      <c r="D58" s="3"/>
+      <c r="A58" s="8">
+        <v>44324</v>
+      </c>
+      <c r="B58" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C58" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="8"/>
@@ -6111,7 +6174,12 @@
       <c r="D1014" s="3"/>
     </row>
     <row r="1015" spans="1:4">
-      <c r="A1015" s="2"/>
+      <c r="A1015" s="8"/>
+      <c r="B1015" s="7"/>
+      <c r="D1015" s="3"/>
+    </row>
+    <row r="1016" spans="1:4">
+      <c r="A1016" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -6123,7 +6191,7 @@
           <x14:formula1>
             <xm:f>Tätigkeiten!$B$2:$B$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C50 C51:C1014</xm:sqref>
+          <xm:sqref>C2:C1015</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6144,10 +6212,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6171,7 +6239,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6179,7 +6247,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6187,7 +6255,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6219,7 +6287,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2">

</xml_diff>